<commit_message>
remove static data and cnvert the framework into TDD
</commit_message>
<xml_diff>
--- a/src/test/java/data/noopCommerceData.xlsx
+++ b/src/test/java/data/noopCommerceData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Self Development\tasks\YassirTask\Yassir\src\test\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E798C1D-4C81-429A-AC63-68EB94B6F990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98CD2EB-37F3-4221-ACFC-6BDB290849E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registrationDataTest" sheetId="1" r:id="rId1"/>
-    <sheet name="registration" sheetId="2" r:id="rId2"/>
+    <sheet name="auto Suggest" sheetId="2" r:id="rId2"/>
+    <sheet name="product checkout" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>firstName</t>
   </si>
@@ -71,6 +72,42 @@
   </si>
   <si>
     <t>123@Aa.4</t>
+  </si>
+  <si>
+    <t>countryName</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>test address</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>Apple MacBook Pro 13-inch</t>
+  </si>
+  <si>
+    <t>partial product name</t>
+  </si>
+  <si>
+    <t>MacB</t>
   </si>
 </sst>
 </file>
@@ -482,42 +519,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9B86FC-5708-44C7-966D-3B8D7FEA7696}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C2" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{C9337770-C6FA-41A2-8346-E3836B92F02A}"/>
-  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F34449-0722-4C03-AB51-77C2557C68BE}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>11659</v>
+      </c>
+      <c r="D2">
+        <v>32445566677</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>